<commit_message>
throw informative error when mismatch in biomarkers from score sheets' names, translation, and consolidation rules
</commit_message>
<xml_diff>
--- a/inst/extdata/tma2/example_pten.xlsx
+++ b/inst/extdata/tma2/example_pten.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/bianca_ribeiro_ubc_ca/Documents/TMAtools/inst/extdata/tma2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{D092F46A-222A-8143-A652-FA1F37E7528F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E4A6F9F-3FA9-49E2-AEF7-1784BCF62BE9}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{D092F46A-222A-8143-A652-FA1F37E7528F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{888373BF-0550-473C-8829-50029569F6D4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TMA map" sheetId="1" r:id="rId1"/>
-    <sheet name="PTEN" sheetId="2" r:id="rId2"/>
+    <sheet name="pten" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -550,7 +550,7 @@
   <dimension ref="C1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>